<commit_message>
Alterando o grid search e os algoritmos de detecção de outlier
</commit_message>
<xml_diff>
--- a/metrics/metricsEE.xlsx
+++ b/metrics/metricsEE.xlsx
@@ -448,7 +448,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5263157894736842</v>
+        <v>0.5131578947368421</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5405405405405406</v>
+        <v>0.5131578947368421</v>
       </c>
     </row>
     <row r="4">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6896551724137931</v>
+        <v>0.6782608695652175</v>
       </c>
     </row>
     <row r="5">
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9523809523809523</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>182.2671518325806</v>
+        <v>384.9190981388092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>